<commit_message>
[MUS]哥特式吸血鬼家具 Gothicstyle Vampire Furniture 업데이트
#746
</commit_message>
<xml_diff>
--- a/Data/[MUS]哥特式吸血鬼家具 Gothicstyle Vampire Furniture - 3102678787/3102678787.xlsx
+++ b/Data/[MUS]哥特式吸血鬼家具 Gothicstyle Vampire Furniture - 3102678787/3102678787.xlsx
@@ -5,15 +5,15 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.7.6\[MUS]哥特式吸血鬼家具 Gothicstyle Vampire Furniture - 3102678787\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\[MUS]哥特式吸血鬼家具 Gothicstyle Vampire Furniture - 3102678787\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CD4D1C-D1F2-4CE6-B208-DD73B258F747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27813FB3-5392-4088-86C8-A87659635D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240409" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_240430" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="568">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -65,6 +65,9 @@
     <t>Castle Floor Tiles</t>
   </si>
   <si>
+    <t>성 타일</t>
+  </si>
+  <si>
     <t>DesignatorDropdownGroupDef+Floor_ScarletMosaic.label</t>
   </si>
   <si>
@@ -74,6 +77,9 @@
     <t>Scarlet Mosaic</t>
   </si>
   <si>
+    <t>스칼럿 모자이크</t>
+  </si>
+  <si>
     <t>DesignatorDropdownGroupDef+Floor_ScarletCarpet.label</t>
   </si>
   <si>
@@ -83,6 +89,9 @@
     <t>Scarlet Carpet</t>
   </si>
   <si>
+    <t>스칼럿 양탄자</t>
+  </si>
+  <si>
     <t>DesignationCategoryDef+Museum_Decoration.label</t>
   </si>
   <si>
@@ -104,6 +113,9 @@
     <t>Added various styles of museum exhibits.</t>
   </si>
   <si>
+    <t>다양한 스타일의 박물관 장식품입니다.</t>
+  </si>
+  <si>
     <t>ResearchProjectDef+Gothicstyle_Vampire_Furniture.label</t>
   </si>
   <si>
@@ -116,6 +128,9 @@
     <t>Gothicstyle Vampire Furniture</t>
   </si>
   <si>
+    <t>고딕 뱀파이어 가구</t>
+  </si>
+  <si>
     <t>ResearchProjectDef+Gothicstyle_Vampire_Furniture.description</t>
   </si>
   <si>
@@ -125,6 +140,9 @@
     <t>The study covers everything from castle structure to tomb decoration。</t>
   </si>
   <si>
+    <t>성 건축부터 무덤 장식까지 모든 것을 아우르는 연구입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Wall.label</t>
   </si>
   <si>
@@ -137,6 +155,9 @@
     <t>Gothic style Wall</t>
   </si>
   <si>
+    <t>고딕 벽</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Wall.description</t>
   </si>
   <si>
@@ -146,6 +167,27 @@
     <t>Gothic style walls with decorative columns and reliefs.</t>
   </si>
   <si>
+    <t>기둥과 부조로 장식된 고딕식 벽입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_WallShootingHole.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_WallShootingHole.label</t>
+  </si>
+  <si>
+    <t>Gothic style Wall Shooting Hole</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_WallShootingHole.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_WallShootingHole.description</t>
+  </si>
+  <si>
+    <t>Gothic style walls with decorative columns and reliefs,Metal window with observation and aiming purpose.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Fence.label</t>
   </si>
   <si>
@@ -155,6 +197,9 @@
     <t>MUS Gothicstyle fence</t>
   </si>
   <si>
+    <t>고딕 울타리</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Fence.description</t>
   </si>
   <si>
@@ -164,6 +209,63 @@
     <t>Strong classical fence, can effectively protect the owner's house.</t>
   </si>
   <si>
+    <t>단단한 고전 양식의 울타리로 집을 효과적으로 보호할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_Hedge.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_Hedge.label</t>
+  </si>
+  <si>
+    <t>MUS Gothicstyle Hedge</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_Hedge.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_Hedge.description</t>
+  </si>
+  <si>
+    <t>The red hedges surround the courtyard in a eerie maze.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_RoseHedge.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_RoseHedge.label</t>
+  </si>
+  <si>
+    <t>Gothicstyle Rose Hedge</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_RoseHedge.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_RoseHedge.description</t>
+  </si>
+  <si>
+    <t>A strange shrub with a rose like appearance, dense and sturdy, with good cover effect, but be careful not to get trapped in the rose maze and die in the sea of fire.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_Barricade.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_Barricade.label</t>
+  </si>
+  <si>
+    <t>Gothicstyle Castle Guardrail</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_Barricade.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_Barricade.description</t>
+  </si>
+  <si>
+    <t>Castle guardrails that can serve as decorations, defensive works, or obstacles.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Column.label</t>
   </si>
   <si>
@@ -173,6 +275,9 @@
     <t>Gothic style Column</t>
   </si>
   <si>
+    <t>고딕 기둥</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Column.description</t>
   </si>
   <si>
@@ -182,6 +287,9 @@
     <t>Four different styles of Gothic columns.</t>
   </si>
   <si>
+    <t>네 종류의 고딕식 기둥입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_WallColumn.label</t>
   </si>
   <si>
@@ -191,6 +299,9 @@
     <t xml:space="preserve">Gothic style Wall column </t>
   </si>
   <si>
+    <t>고딕 벽 기둥 (측면)</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_WallColumn.description</t>
   </si>
   <si>
@@ -200,6 +311,9 @@
     <t>Gothic wall columns are usually used to support arches, but as decorative parts of the wall, they themselves do not have support capacity.</t>
   </si>
   <si>
+    <t>고딕 벽 기둥은 주로 아치를 지탱하는 데 사용되지만 벽의 장식부로서 천장을 받칠 수는 없습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_WallColumnFront.label</t>
   </si>
   <si>
@@ -209,6 +323,9 @@
     <t>Gothic style Wall column Front</t>
   </si>
   <si>
+    <t>고딕 벽 기둥 (전면)</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_WallColumnFront.description</t>
   </si>
   <si>
@@ -224,6 +341,9 @@
     <t>Gothic style Arch</t>
   </si>
   <si>
+    <t>고딕 아치</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Arch.description</t>
   </si>
   <si>
@@ -233,6 +353,45 @@
     <t>Gothic arch with good load-bearing characteristics, but as decorative parts of the wall, they themselves do not have support capacity.</t>
   </si>
   <si>
+    <t>하중을 잘 견디는 고딕식 아치입니다. 벽의 장식부로서 천장을 받칠 수는 없습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_SmallArch.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_SmallArch.label</t>
+  </si>
+  <si>
+    <t>Gothic style Small Arch</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_SmallArch.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_SmallArch.description</t>
+  </si>
+  <si>
+    <t>Gothic small arch with good load-bearing characteristics, but as decorative parts of the wall, they themselves do not have support capacity.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_CourtyardArch.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_CourtyardArch.label</t>
+  </si>
+  <si>
+    <t>Gothic style Courtyard Arch</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_CourtyardArch.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_CourtyardArch.description</t>
+  </si>
+  <si>
+    <t>An arch composed of hedges and wreaths, responsible for guiding lost people through the vast maze of roses.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_FlyingButtress.label</t>
   </si>
   <si>
@@ -242,6 +401,9 @@
     <t>Gothic style Flying Buttress</t>
   </si>
   <si>
+    <t>고딕 부벽</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_FlyingButtress.description</t>
   </si>
   <si>
@@ -251,6 +413,9 @@
     <t>A building structure that serves as a support.</t>
   </si>
   <si>
+    <t>지지대 역할을 할 수 있는 구조물입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_door.label</t>
   </si>
   <si>
@@ -260,6 +425,9 @@
     <t>Gothicstyle door</t>
   </si>
   <si>
+    <t>고딕 문</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_door.description</t>
   </si>
   <si>
@@ -269,6 +437,9 @@
     <t>Gothic door with decorative patterns on it.</t>
   </si>
   <si>
+    <t>장식 무늬가 있는 고딕식 문입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Fencedoor.label</t>
   </si>
   <si>
@@ -278,6 +449,9 @@
     <t>Gothicstyle Fence door</t>
   </si>
   <si>
+    <t>고딕 울타리 문</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Fencedoor.description</t>
   </si>
   <si>
@@ -287,6 +461,63 @@
     <t>Heavy and cold.</t>
   </si>
   <si>
+    <t>무겁고 차갑습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_Autodoor.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_Autodoor.label</t>
+  </si>
+  <si>
+    <t>Gothicstyle Autodoor</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_Autodoor.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_Autodoor.description</t>
+  </si>
+  <si>
+    <t>"Of course, it's powered by electricity, not a vampire trick."</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_CastleDoor.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_CastleDoor.label</t>
+  </si>
+  <si>
+    <t>Gothicstyle Castle Door</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_CastleDoor.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_CastleDoor.description</t>
+  </si>
+  <si>
+    <t>A heavy city gate reinforced with steel.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_CastleAutoDoor.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_CastleAutoDoor.label</t>
+  </si>
+  <si>
+    <t>Gothicstyle Castle Auto Door</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_CastleAutoDoor.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_CastleAutoDoor.description</t>
+  </si>
+  <si>
+    <t>Although it is very heavy, the built-in mechanical equipment can greatly reduce the difficulty of the door opener.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_BloodCoffins.label</t>
   </si>
   <si>
@@ -296,6 +527,9 @@
     <t>Gothicstyle Blood Coffins</t>
   </si>
   <si>
+    <t>고딕 핏빛 관</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_BloodCoffins.description</t>
   </si>
   <si>
@@ -305,6 +539,9 @@
     <t>The cursed coffin statue, it makes people shudder.</t>
   </si>
   <si>
+    <t>저주받은 관 모양의 조각상으로 사람들을 공포에 휩싸이게 만듭니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_ProfaneBloodCoffins.label</t>
   </si>
   <si>
@@ -314,6 +551,9 @@
     <t>Gothicstyle Profane Blood Coffins</t>
   </si>
   <si>
+    <t>고딕 모독적인 핏빛 관</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_ProfaneBloodCoffins.description</t>
   </si>
   <si>
@@ -329,6 +569,9 @@
     <t>Gothicstyle Tomb Statue</t>
   </si>
   <si>
+    <t>고딕 해골상</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_TombStatue.description</t>
   </si>
   <si>
@@ -338,6 +581,9 @@
     <t>Everywhere is full of skeletons.</t>
   </si>
   <si>
+    <t>해골투성이입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Window.label</t>
   </si>
   <si>
@@ -347,6 +593,9 @@
     <t>Gothic Blood Window</t>
   </si>
   <si>
+    <t>고딕 핏빛 창문</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Window.description</t>
   </si>
   <si>
@@ -356,6 +605,9 @@
     <t>A window woven into fiberglass with blood,Even in the dark underground, it emits an ominous red light.</t>
   </si>
   <si>
+    <t>피를 머금은 유리섬유로 만든 창문입니다. 어두운 지하에서도 불길한 붉은 빛을 내뿜습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Pendant.label</t>
   </si>
   <si>
@@ -365,6 +617,9 @@
     <t>Gothic style Pendant</t>
   </si>
   <si>
+    <t>고딕 샹들리에</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Pendant.description</t>
   </si>
   <si>
@@ -374,6 +629,27 @@
     <t>Using blood clotted candles to illuminate, emitting a cool red light that is neither heat nor extinguished.</t>
   </si>
   <si>
+    <t>피를 굳혀 만든 양초로 불을 밝히며, 열을 내지도 꺼지지도 않는 차가운 붉은 빛을 발산합니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_SmallPendant.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_SmallPendant.label</t>
+  </si>
+  <si>
+    <t>Gothic style Small Pendant</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_SmallPendant.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_SmallPendant.description</t>
+  </si>
+  <si>
+    <t>The strange creature in the cage, its eyes flickering with red light, shaking the cage and making a creaking sound.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Candlestick.label</t>
   </si>
   <si>
@@ -383,6 +659,9 @@
     <t>Gothicstyle Candlestick</t>
   </si>
   <si>
+    <t>고딕 스탠드 촛대</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Candlestick.description</t>
   </si>
   <si>
@@ -398,6 +677,9 @@
     <t>Gothicstyle Candle</t>
   </si>
   <si>
+    <t>고딕 촛대</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Candle.description</t>
   </si>
   <si>
@@ -413,6 +695,9 @@
     <t>Gothicstyle Wall Candle</t>
   </si>
   <si>
+    <t>고딕 벽 촛대</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_WallCandle.description</t>
   </si>
   <si>
@@ -428,6 +713,9 @@
     <t>Gothicstyle Heavy Fireplace</t>
   </si>
   <si>
+    <t>고딕 벽난로</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Fireplace.description</t>
   </si>
   <si>
@@ -437,6 +725,9 @@
     <t>"Don't be afraid, come closer, this fire isn't hot at all," and a hallucinatory flame burned in the lobby fireplace, making the space seem unusually cold.</t>
   </si>
   <si>
+    <t>"두려워하지 말고, 가까이 오렴. 이 불은 전혀 뜨겁지 않단다." 로비 벽난로에서 불꽃 모양의 환영이 타오르며 방 안을 유난히 쌀쌀하게 만듭니다.</t>
+  </si>
+  <si>
     <t>TerrainDef+RedScarletMosaic.description</t>
   </si>
   <si>
@@ -449,6 +740,9 @@
     <t>The mosaic floor, stained red with blood, seems to be like a living creature that will nibble at the dirt attached to the surface.</t>
   </si>
   <si>
+    <t>피로 붉게 물든 모자이크 바닥입니다. 표면에 먼지라도 떨어지면 마치 살아있는 생명체처럼 잠식해 먹어치워 버립니다.</t>
+  </si>
+  <si>
     <t>TerrainDef+RedScarletMosaic.label</t>
   </si>
   <si>
@@ -458,6 +752,9 @@
     <t>Red Scarlet Mosaic</t>
   </si>
   <si>
+    <t>스칼럿 모자이크 (빨간색)</t>
+  </si>
+  <si>
     <t>TerrainDef+YellowScarletMosaic.description</t>
   </si>
   <si>
@@ -473,6 +770,9 @@
     <t>Yellow Scarlet Mosaic</t>
   </si>
   <si>
+    <t>스칼럿 모자이크 (노란색)</t>
+  </si>
+  <si>
     <t>TerrainDef+GreenScarletMosaic.description</t>
   </si>
   <si>
@@ -488,6 +788,9 @@
     <t>Green Scarlet Mosaic</t>
   </si>
   <si>
+    <t>스칼럿 모자이크 (녹색)</t>
+  </si>
+  <si>
     <t>TerrainDef+BlueScarletMosaic.description</t>
   </si>
   <si>
@@ -503,6 +806,9 @@
     <t>Blue Scarlet Mosaic</t>
   </si>
   <si>
+    <t>스칼럿 모자이크 (파란색)</t>
+  </si>
+  <si>
     <t>TerrainDef+WhiteScarletMosaic.description</t>
   </si>
   <si>
@@ -518,6 +824,9 @@
     <t>White Scarlet Mosaic</t>
   </si>
   <si>
+    <t>스칼럿 모자이크 (흰색)</t>
+  </si>
+  <si>
     <t>TerrainDef+BlackScarletMosaic.description</t>
   </si>
   <si>
@@ -533,6 +842,9 @@
     <t>Black Scarlet Mosaic</t>
   </si>
   <si>
+    <t>스칼럿 모자이크 (검은색)</t>
+  </si>
+  <si>
     <t>TerrainDef+RedScarletCarpet.description</t>
   </si>
   <si>
@@ -542,6 +854,9 @@
     <t>A carpet woven with blood, with strange patterns that make viewers feel dizzy and beautiful.</t>
   </si>
   <si>
+    <t>피로 엮은 양탄자입니다. 보는 이들을 어지럽게 하면서도 아름답다는 느낌이 드는 기묘한 무늬가 있습니다.</t>
+  </si>
+  <si>
     <t>TerrainDef+RedScarletCarpet.label</t>
   </si>
   <si>
@@ -551,6 +866,9 @@
     <t>Red Scarlet Carpet</t>
   </si>
   <si>
+    <t>스칼럿 양탄자 (빨간색)</t>
+  </si>
+  <si>
     <t>TerrainDef+YellowScarletCarpet.description</t>
   </si>
   <si>
@@ -566,6 +884,9 @@
     <t>Yellow Scarlet Carpet</t>
   </si>
   <si>
+    <t>스칼럿 양탄자 (노란색)</t>
+  </si>
+  <si>
     <t>TerrainDef+GreenScarletCarpet.description</t>
   </si>
   <si>
@@ -581,6 +902,9 @@
     <t>Green Scarlet Carpet</t>
   </si>
   <si>
+    <t>스칼럿 양탄자 (녹색)</t>
+  </si>
+  <si>
     <t>TerrainDef+BlueScarletCarpet.description</t>
   </si>
   <si>
@@ -596,6 +920,9 @@
     <t>Blue Scarlet Carpet</t>
   </si>
   <si>
+    <t>스칼럿 양탄자 (파란색)</t>
+  </si>
+  <si>
     <t>TerrainDef+WhiteScarletCarpet.description</t>
   </si>
   <si>
@@ -611,6 +938,9 @@
     <t>White Scarlet Carpet</t>
   </si>
   <si>
+    <t>스칼럿 양탄자 (흰색)</t>
+  </si>
+  <si>
     <t>TerrainDef+BlackScarletCarpet.description</t>
   </si>
   <si>
@@ -626,6 +956,9 @@
     <t>Black Scarlet Carpet</t>
   </si>
   <si>
+    <t>스칼럿 양탄자 (검은색)</t>
+  </si>
+  <si>
     <t>TerrainDef+CastleFloorTilesSandstone.description</t>
   </si>
   <si>
@@ -635,6 +968,9 @@
     <t>Using simple cut rough stone paving, suitable for large-scale paving but lacking aesthetic appeal.</t>
   </si>
   <si>
+    <t>간단하게 자른 거친 석재 블록을 사용하여 대규모 길 포장에는 적합하지만 미적 측면은 부족합니다.</t>
+  </si>
+  <si>
     <t>TerrainDef+CastleFloorTilesSandstone.label</t>
   </si>
   <si>
@@ -644,6 +980,9 @@
     <t>Castle Floor Tiles sandstone</t>
   </si>
   <si>
+    <t>사암 성 타일</t>
+  </si>
+  <si>
     <t>TerrainDef+CastleFloorTilesGranite.description</t>
   </si>
   <si>
@@ -659,6 +998,9 @@
     <t>Castle Floor Tiles granite</t>
   </si>
   <si>
+    <t>화강암 성 타일</t>
+  </si>
+  <si>
     <t>TerrainDef+CastleFloorTilesLimestone.description</t>
   </si>
   <si>
@@ -674,6 +1016,9 @@
     <t>Castle Floor Tiles limestone</t>
   </si>
   <si>
+    <t>석회암 성 타일</t>
+  </si>
+  <si>
     <t>TerrainDef+CastleFloorTilesSlate.description</t>
   </si>
   <si>
@@ -689,6 +1034,9 @@
     <t>Castle Floor Tiles slate</t>
   </si>
   <si>
+    <t>점판암 성 타일</t>
+  </si>
+  <si>
     <t>TerrainDef+CastleFloorTilesMarble.description</t>
   </si>
   <si>
@@ -704,6 +1052,9 @@
     <t>Castle Floor Tiles marble</t>
   </si>
   <si>
+    <t>대리석 성 타일</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_DecorativeArmor.label</t>
   </si>
   <si>
@@ -713,6 +1064,9 @@
     <t>Gothicstyle Decorative Armor</t>
   </si>
   <si>
+    <t>고딕 갑옷상</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_DecorativeArmor.description</t>
   </si>
   <si>
@@ -722,6 +1076,9 @@
     <t>A set of decorative armor equipped with a spear to guard its owner's castle.</t>
   </si>
   <si>
+    <t>주인의 성을 지키기 위해 창으로 무장한 장식용 갑옷상입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_MonsterStatueSmall.label</t>
   </si>
   <si>
@@ -731,6 +1088,9 @@
     <t>Gothicstyle Gargoyle Statue</t>
   </si>
   <si>
+    <t>고딕 가고일상</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_MonsterStatueSmall.description</t>
   </si>
   <si>
@@ -740,6 +1100,9 @@
     <t>A statue of a loyal gargoyle.</t>
   </si>
   <si>
+    <t>충성스러운 가고일의 조각상입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_HeavyCurtain.label</t>
   </si>
   <si>
@@ -749,6 +1112,9 @@
     <t>Gothicstyle Heavy Curtain</t>
   </si>
   <si>
+    <t>고딕 커튼</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_HeavyCurtain.description</t>
   </si>
   <si>
@@ -758,6 +1124,27 @@
     <t>Thick curtains are usually thought to block out light, and you don't want that sunlight on your skin.</t>
   </si>
   <si>
+    <t>두꺼운 커튼은 일반적으로 빛을 차단하는 데 효과적입니다. 당신도 피부가 햇빛에 노출되는 걸 원하진 않겠죠.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_ThinCurtain.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_ThinCurtain.label</t>
+  </si>
+  <si>
+    <t>Gothicstyle Thin Curtain</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_ThinCurtain.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_ThinCurtain.description</t>
+  </si>
+  <si>
+    <t>It is smaller and lighter, with lower costs, and a 50% higher probability of being exposed to sunlight.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Flowerpot.label</t>
   </si>
   <si>
@@ -767,6 +1154,9 @@
     <t>Gothicstyle Flowerpot</t>
   </si>
   <si>
+    <t>고딕 화분</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Flowerpot.description</t>
   </si>
   <si>
@@ -776,6 +1166,9 @@
     <t>Blood-colored flowers decorated the dim corridor, and the air was filled with the intoxicating scent of flowers.</t>
   </si>
   <si>
+    <t>핏빛으로 물든 꽃들이 어둑어둑한 복도를 장식했고, 공기 중엔 취할 듯한 꽃향기가 가득했습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_DesktopDecoration.label</t>
   </si>
   <si>
@@ -785,6 +1178,9 @@
     <t>Gothicstyle Desktop Decoration</t>
   </si>
   <si>
+    <t>고딕 탁자 장식</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_DesktopDecoration.description</t>
   </si>
   <si>
@@ -794,6 +1190,9 @@
     <t>Maybe it's just a bunch of roses, maybe it's a pot of wine, maybe it's eyes staring in the dark.</t>
   </si>
   <si>
+    <t>이 장식은 장미 여러 송이일 수도, 병에 담긴 와인일 수도, 어쩌면 어둠 속을 응시하는 눈일 수도 있습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_GrandfatherClock.label</t>
   </si>
   <si>
@@ -803,6 +1202,9 @@
     <t>Gothicstyle Grandfather Clock</t>
   </si>
   <si>
+    <t>고딕 괘종시계</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_GrandfatherClock.description</t>
   </si>
   <si>
@@ -812,6 +1214,9 @@
     <t>If you hear the clock strike thirteen in the middle of the night, don't try to fix it.</t>
   </si>
   <si>
+    <t>한밤중에 시계가 13시를 알리는 소리가 들린다면 고치려 하지 마세요.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_OilPainting.label</t>
   </si>
   <si>
@@ -821,6 +1226,9 @@
     <t>Gothic Oil Painting</t>
   </si>
   <si>
+    <t>고딕 유화 액자</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_OilPainting.description</t>
   </si>
   <si>
@@ -830,6 +1238,27 @@
     <t>A still life. It looks rather boring.</t>
   </si>
   <si>
+    <t>정물화입니다. 딱히 흥미를 끄는 점은 없습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_EerieOilPainting.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_EerieOilPainting.label</t>
+  </si>
+  <si>
+    <t>Gothic Eerie Oil Painting</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_EerieOilPainting.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_EerieOilPainting.description</t>
+  </si>
+  <si>
+    <t>An uninteresting still life painting from a mediocre painter who has long disappeared. Visitors always complain that when they share a room with the painting, they always feel like something is peeking at them.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_DoubleSofa.label</t>
   </si>
   <si>
@@ -839,6 +1268,9 @@
     <t>Gothicstyle Double Sofa</t>
   </si>
   <si>
+    <t>고딕 큰 소파</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_DoubleSofa.description</t>
   </si>
   <si>
@@ -848,6 +1280,9 @@
     <t>An elegant double sofa made of comfortable fabric and leather.</t>
   </si>
   <si>
+    <t>편안한 원단과 가죽으로 제작된 우아한 큰 소파입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Sofa.label</t>
   </si>
   <si>
@@ -857,6 +1292,9 @@
     <t>Gothicstyle Sofa</t>
   </si>
   <si>
+    <t>고딕 소파</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Sofa.description</t>
   </si>
   <si>
@@ -866,6 +1304,9 @@
     <t>An elegant sofa made of comfortable fabric and leather.</t>
   </si>
   <si>
+    <t>편안한 원단과 가죽으로 제작된 우아한 소파입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_DiningChair.label</t>
   </si>
   <si>
@@ -875,6 +1316,9 @@
     <t>Gothicstyle DiningChair</t>
   </si>
   <si>
+    <t>고딕 식탁 의자</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_DiningChair.description</t>
   </si>
   <si>
@@ -884,6 +1328,9 @@
     <t>A Gothic dining chair, decorated with a slightly intricate grain, in the hope that visitors visiting on rainy nights will like them.</t>
   </si>
   <si>
+    <t>다소 복잡한 무늬로 장식된 고딕식 식탁 의자입니다. 비 오는 밤에 찾아오는 손님들의 마음에 들었으면 좋겠습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_TableMini.label</t>
   </si>
   <si>
@@ -893,6 +1340,9 @@
     <t>Gothicstyle Table Mini</t>
   </si>
   <si>
+    <t>고딕 테이블 (1x1)</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_TableMini.description</t>
   </si>
   <si>
@@ -902,6 +1352,9 @@
     <t>A nice little table. Put up the candlesticks. I hope you enjoy your candlelit dinner.</t>
   </si>
   <si>
+    <t>좋은 미니 테이블입니다. 촛대를 올려 보세요. 이제 촛불로 분위기를 낸 맛있는 저녁 식사를 하시길 바랍니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_TableSmall.label</t>
   </si>
   <si>
@@ -911,6 +1364,9 @@
     <t>Gothicstyle Table Small</t>
   </si>
   <si>
+    <t>고딕 테이블 (2x1)</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_TableSmall.description</t>
   </si>
   <si>
@@ -920,6 +1376,9 @@
     <t>A good sized table, perfect for most occasions, but you don't remember where this tablecloth came from.</t>
   </si>
   <si>
+    <t>여러 가지 용도로 쓸 수 있는 적당한 크기의 테이블입니다. 테이블보가 어디에서 왔는지는 의문입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Table.label</t>
   </si>
   <si>
@@ -929,6 +1388,9 @@
     <t>Gothicstyle Table</t>
   </si>
   <si>
+    <t>고딕 테이블 (2x2)</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Table.description</t>
   </si>
   <si>
@@ -938,6 +1400,9 @@
     <t>Spacious table, suitable for chatting with your friends, but please do not bet your head with the devil.</t>
   </si>
   <si>
+    <t>친구들과 모여 이야기하기에 좋은 넓은 테이블입니다. 여기서 악마와 자신의 머리를 걸고 내기를 하면 안 됩니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_TableBig.label</t>
   </si>
   <si>
@@ -947,6 +1412,9 @@
     <t>Gothicstyle Table Big</t>
   </si>
   <si>
+    <t>고딕 테이블 (4x2)</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_TableBig.description</t>
   </si>
   <si>
@@ -956,6 +1424,9 @@
     <t>The huge table, which is the centerpiece of the banquet, treats the guests well, hoping they start with the same number of people as they finish.</t>
   </si>
   <si>
+    <t>연회장 중심에 놓일 만한 거대한 테이블입니다. 손님들을 잘 대해 주세요. 부디 연회가 시작됐을 때와 끝났을 때의 인원수가 같기를 바랍니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_SmallRoundTable.label</t>
   </si>
   <si>
@@ -965,6 +1436,9 @@
     <t>Gothicstyle Small Round Table</t>
   </si>
   <si>
+    <t>고딕 와인 테이블 (1x1)</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_SmallRoundTable.description</t>
   </si>
   <si>
@@ -974,6 +1448,9 @@
     <t>"You should warm yourself up with this nice bottle of wine. I wish you good health".</t>
   </si>
   <si>
+    <t>"이 멋진 와인 한 잔으로 몸이라도 녹이렴. 네가 건강하길 바란단다."</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Cupboard.label</t>
   </si>
   <si>
@@ -983,6 +1460,9 @@
     <t>Gothicstyle Cupboard</t>
   </si>
   <si>
+    <t>고딕 찬장</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Cupboard.description</t>
   </si>
   <si>
@@ -992,6 +1472,9 @@
     <t>Little stuff, old photos, some red liquid bottles. It seems that the most meaningless things in the house are concentrated in this cupboard.</t>
   </si>
   <si>
+    <t>작은 물건들, 오래된 사진, 빨간 액체가 든 병들... 집안에서 가장 의미없는 것들이 전부 이 찬장 안에 들어 있는 것 같습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Wardrobe.label</t>
   </si>
   <si>
@@ -1001,6 +1484,9 @@
     <t>Gothicstyle Wardrobe</t>
   </si>
   <si>
+    <t>고딕 옷장</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Wardrobe.description</t>
   </si>
   <si>
@@ -1010,6 +1496,9 @@
     <t>There are no eyes in the closet to spy on you, the back of the closet is of course solid.</t>
   </si>
   <si>
+    <t>옷장 안에 슬쩍 이쪽을 훔쳐보는 눈 따위는 없습니다. 뒷면도 당연히 막혀 있고요.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Mirror.label</t>
   </si>
   <si>
@@ -1019,6 +1508,9 @@
     <t>Gothicstyle Mirror</t>
   </si>
   <si>
+    <t>고딕 거울</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Mirror.description</t>
   </si>
   <si>
@@ -1028,6 +1520,9 @@
     <t>Because every mirror is covered in red paint, you can't see me in the mirror at all.</t>
   </si>
   <si>
+    <t>표면이 빨간 페인트로 칠해져 있어 아무것도 비치지 않습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_BedsideTable.label</t>
   </si>
   <si>
@@ -1037,6 +1532,9 @@
     <t>Gothicstyle Bedside Table</t>
   </si>
   <si>
+    <t>고딕 협탁</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_BedsideTable.description</t>
   </si>
   <si>
@@ -1046,6 +1544,9 @@
     <t>The drawer contains a set of garlic, stakes and mallets so you can sleep at night. And watch your toes, please.</t>
   </si>
   <si>
+    <t>서랍에는 야간 수면을 위한 마늘과 말뚝, 그리고 망치 세트가 들어있습니다. 발가락을 부딪히지 않게 조심하세요.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Bed.label</t>
   </si>
   <si>
@@ -1055,6 +1556,9 @@
     <t>Gothicstyle Bed</t>
   </si>
   <si>
+    <t>고딕 침대</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_Bed.description</t>
   </si>
   <si>
@@ -1064,6 +1568,9 @@
     <t>“Soft and comfortable, you can sleep on it as peacefully as the dead, of course I'm only speaking metaphorically, don't take it personally“.</t>
   </si>
   <si>
+    <t>“부드럽고 편안한 침대란다. 죽은 사람처럼 평온하게 잘 수 있지. 물론 비유일 뿐이니, 너무 진지하게 받아들이진 말렴.“</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_DoubleBed.label</t>
   </si>
   <si>
@@ -1073,6 +1580,9 @@
     <t>Gothicstyle Double Bed</t>
   </si>
   <si>
+    <t>고딕 큰 침대</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_DoubleBed.description</t>
   </si>
   <si>
@@ -1082,6 +1592,9 @@
     <t>A big, solid bed, full of material, soft as velvet.</t>
   </si>
   <si>
+    <t>크고 견고한 침대입니다. 풍부한 재료로 만들어져 벨벳처럼 부드럽습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_CoffinBed.label</t>
   </si>
   <si>
@@ -1091,6 +1604,9 @@
     <t>Gothicstyle Coffin Bed</t>
   </si>
   <si>
+    <t>고딕 수면관</t>
+  </si>
+  <si>
     <t>ThingDef+MUS_Gothicstyle_CoffinBed.description</t>
   </si>
   <si>
@@ -1103,304 +1619,124 @@
     <t>마치 죽은 사람이 된 것 같이 평온한 수면 경험을 선사할 수 있습니다.</t>
   </si>
   <si>
-    <t>고딕 수면관</t>
-  </si>
-  <si>
-    <t>크고 견고한 침대입니다. 풍부한 재료로 만들어져 벨벳처럼 부드럽습니다.</t>
-  </si>
-  <si>
-    <t>고딕 큰 침대</t>
-  </si>
-  <si>
-    <t>“부드럽고 편안한 침대란다. 죽은 사람처럼 평온하게 잘 수 있지. 물론 비유일 뿐이니, 너무 진지하게 받아들이진 말렴.“</t>
-  </si>
-  <si>
-    <t>고딕 침대</t>
-  </si>
-  <si>
-    <t>서랍에는 야간 수면을 위한 마늘과 말뚝, 그리고 망치 세트가 들어있습니다. 발가락을 부딪히지 않게 조심하세요.</t>
-  </si>
-  <si>
-    <t>고딕 협탁</t>
-  </si>
-  <si>
-    <t>표면이 빨간 페인트로 칠해져 있어 아무것도 비치지 않습니다.</t>
-  </si>
-  <si>
-    <t>고딕 거울</t>
-  </si>
-  <si>
-    <t>옷장 안에 슬쩍 이쪽을 훔쳐보는 눈 따위는 없습니다. 뒷면도 당연히 막혀 있고요.</t>
-  </si>
-  <si>
-    <t>고딕 옷장</t>
-  </si>
-  <si>
-    <t>작은 물건들, 오래된 사진, 빨간 액체가 든 병들... 집안에서 가장 의미없는 것들이 전부 이 찬장 안에 들어 있는 것 같습니다.</t>
-  </si>
-  <si>
-    <t>고딕 찬장</t>
-  </si>
-  <si>
-    <t>"이 멋진 와인 한 잔으로 몸이라도 녹이렴. 네가 건강하길 바란단다."</t>
-  </si>
-  <si>
-    <t>고딕 와인 테이블 (1x1)</t>
-  </si>
-  <si>
-    <t>연회장 중심에 놓일 만한 거대한 테이블입니다. 손님들을 잘 대해 주세요. 부디 연회가 시작됐을 때와 끝났을 때의 인원수가 같기를 바랍니다.</t>
-  </si>
-  <si>
-    <t>고딕 테이블 (4x2)</t>
-  </si>
-  <si>
-    <t>친구들과 모여 이야기하기에 좋은 넓은 테이블입니다. 여기서 악마와 자신의 머리를 걸고 내기를 하면 안 됩니다.</t>
-  </si>
-  <si>
-    <t>고딕 테이블 (2x2)</t>
-  </si>
-  <si>
-    <t>여러 가지 용도로 쓸 수 있는 적당한 크기의 테이블입니다. 테이블보가 어디에서 왔는지는 의문입니다.</t>
-  </si>
-  <si>
-    <t>고딕 테이블 (2x1)</t>
-  </si>
-  <si>
-    <t>좋은 미니 테이블입니다. 촛대를 올려 보세요. 이제 촛불로 분위기를 낸 맛있는 저녁 식사를 하시길 바랍니다.</t>
-  </si>
-  <si>
-    <t>고딕 테이블 (1x1)</t>
-  </si>
-  <si>
-    <t>다소 복잡한 무늬로 장식된 고딕식 식탁 의자입니다. 비 오는 밤에 찾아오는 손님들의 마음에 들었으면 좋겠습니다.</t>
-  </si>
-  <si>
-    <t>고딕 식탁 의자</t>
-  </si>
-  <si>
-    <t>편안한 원단과 가죽으로 제작된 우아한 소파입니다.</t>
-  </si>
-  <si>
-    <t>고딕 소파</t>
-  </si>
-  <si>
-    <t>편안한 원단과 가죽으로 제작된 우아한 큰 소파입니다.</t>
-  </si>
-  <si>
-    <t>고딕 큰 소파</t>
-  </si>
-  <si>
-    <t>정물화입니다. 딱히 흥미를 끄는 점은 없습니다.</t>
-  </si>
-  <si>
-    <t>고딕 유화 액자</t>
-  </si>
-  <si>
-    <t>한밤중에 시계가 13시를 알리는 소리가 들린다면 고치려 하지 마세요.</t>
-  </si>
-  <si>
-    <t>고딕 괘종시계</t>
-  </si>
-  <si>
-    <t>이 장식은 장미 여러 송이일 수도, 병에 담긴 와인일 수도, 어쩌면 어둠 속을 응시하는 눈일 수도 있습니다.</t>
-  </si>
-  <si>
-    <t>고딕 탁자 장식</t>
-  </si>
-  <si>
-    <t>핏빛으로 물든 꽃들이 어둑어둑한 복도를 장식했고, 공기 중엔 취할 듯한 꽃향기가 가득했습니다.</t>
-  </si>
-  <si>
-    <t>고딕 화분</t>
-  </si>
-  <si>
-    <t>두꺼운 커튼은 일반적으로 빛을 차단하는 데 효과적입니다. 당신도 피부가 햇빛에 노출되는 걸 원하진 않겠죠.</t>
-  </si>
-  <si>
-    <t>고딕 커튼</t>
-  </si>
-  <si>
-    <t>충성스러운 가고일의 조각상입니다.</t>
-  </si>
-  <si>
-    <t>고딕 가고일상</t>
-  </si>
-  <si>
-    <t>주인의 성을 지키기 위해 창으로 무장한 장식용 갑옷상입니다.</t>
-  </si>
-  <si>
-    <t>고딕 갑옷상</t>
-  </si>
-  <si>
-    <t>"두려워하지 말고, 가까이 오렴. 이 불은 전혀 뜨겁지 않단다." 로비 벽난로에서 불꽃 모양의 환영이 타오르며 방 안을 유난히 쌀쌀하게 만듭니다.</t>
-  </si>
-  <si>
-    <t>고딕 벽난로</t>
-  </si>
-  <si>
-    <t>피를 굳혀 만든 양초로 불을 밝히며, 열을 내지도 꺼지지도 않는 차가운 붉은 빛을 발산합니다.</t>
-  </si>
-  <si>
-    <t>고딕 벽 촛대</t>
-  </si>
-  <si>
-    <t>고딕 촛대</t>
-  </si>
-  <si>
-    <t>고딕 스탠드 촛대</t>
-  </si>
-  <si>
-    <t>고딕 샹들리에</t>
-  </si>
-  <si>
-    <t>피를 머금은 유리섬유로 만든 창문입니다. 어두운 지하에서도 불길한 붉은 빛을 내뿜습니다.</t>
-  </si>
-  <si>
-    <t>고딕 핏빛 창문</t>
-  </si>
-  <si>
-    <t>해골투성이입니다.</t>
-  </si>
-  <si>
-    <t>고딕 해골상</t>
-  </si>
-  <si>
-    <t>저주받은 관 모양의 조각상으로 사람들을 공포에 휩싸이게 만듭니다.</t>
-  </si>
-  <si>
-    <t>고딕 모독적인 핏빛 관</t>
-  </si>
-  <si>
-    <t>고딕 핏빛 관</t>
-  </si>
-  <si>
-    <t>무겁고 차갑습니다.</t>
-  </si>
-  <si>
-    <t>고딕 울타리 문</t>
-  </si>
-  <si>
-    <t>장식 무늬가 있는 고딕식 문입니다.</t>
-  </si>
-  <si>
-    <t>고딕 문</t>
-  </si>
-  <si>
-    <t>지지대 역할을 할 수 있는 구조물입니다.</t>
-  </si>
-  <si>
-    <t>고딕 부벽</t>
-  </si>
-  <si>
-    <t>하중을 잘 견디는 고딕식 아치입니다. 벽의 장식부로서 천장을 받칠 수는 없습니다.</t>
-  </si>
-  <si>
-    <t>고딕 아치</t>
-  </si>
-  <si>
-    <t>고딕 벽 기둥은 주로 아치를 지탱하는 데 사용되지만 벽의 장식부로서 천장을 받칠 수는 없습니다.</t>
-  </si>
-  <si>
-    <t>고딕 벽 기둥 (전면)</t>
-  </si>
-  <si>
-    <t>고딕 벽 기둥 (측면)</t>
-  </si>
-  <si>
-    <t>네 종류의 고딕식 기둥입니다.</t>
-  </si>
-  <si>
-    <t>고딕 기둥</t>
-  </si>
-  <si>
-    <t>단단한 고전 양식의 울타리로 집을 효과적으로 보호할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>고딕 울타리</t>
-  </si>
-  <si>
-    <t>기둥과 부조로 장식된 고딕식 벽입니다.</t>
-  </si>
-  <si>
-    <t>고딕 벽</t>
-  </si>
-  <si>
-    <t>간단하게 자른 거친 석재 블록을 사용하여 대규모 길 포장에는 적합하지만 미적 측면은 부족합니다.</t>
-  </si>
-  <si>
-    <t>대리석 성 타일</t>
-  </si>
-  <si>
-    <t>점판암 성 타일</t>
-  </si>
-  <si>
-    <t>석회암 성 타일</t>
-  </si>
-  <si>
-    <t>화강암 성 타일</t>
-  </si>
-  <si>
-    <t>사암 성 타일</t>
-  </si>
-  <si>
-    <t>피로 엮은 양탄자입니다. 보는 이들을 어지럽게 하면서도 아름답다는 느낌이 드는 기묘한 무늬가 있습니다.</t>
-  </si>
-  <si>
-    <t>스칼럿 양탄자 (검은색)</t>
-  </si>
-  <si>
-    <t>스칼럿 양탄자 (흰색)</t>
-  </si>
-  <si>
-    <t>스칼럿 양탄자 (파란색)</t>
-  </si>
-  <si>
-    <t>스칼럿 양탄자 (녹색)</t>
-  </si>
-  <si>
-    <t>스칼럿 양탄자 (노란색)</t>
-  </si>
-  <si>
-    <t>스칼럿 양탄자 (빨간색)</t>
-  </si>
-  <si>
-    <t>피로 붉게 물든 모자이크 바닥입니다. 표면에 먼지라도 떨어지면 마치 살아있는 생명체처럼 잠식해 먹어치워 버립니다.</t>
-  </si>
-  <si>
-    <t>스칼럿 모자이크 (검은색)</t>
-  </si>
-  <si>
-    <t>스칼럿 모자이크 (흰색)</t>
-  </si>
-  <si>
-    <t>스칼럿 모자이크 (파란색)</t>
-  </si>
-  <si>
-    <t>스칼럿 모자이크 (녹색)</t>
-  </si>
-  <si>
-    <t>스칼럿 모자이크 (노란색)</t>
-  </si>
-  <si>
-    <t>스칼럿 모자이크 (빨간색)</t>
-  </si>
-  <si>
-    <t>성 건축부터 무덤 장식까지 모든 것을 아우르는 연구입니다.</t>
-  </si>
-  <si>
-    <t>고딕 뱀파이어 가구</t>
-  </si>
-  <si>
-    <t>스칼럿 양탄자</t>
-  </si>
-  <si>
-    <t>스칼럿 모자이크</t>
-  </si>
-  <si>
-    <t>성 타일</t>
-  </si>
-  <si>
-    <t>다양한 스타일의 박물관 장식품입니다.</t>
+    <t>ThingDef+MUS_Gothicstyle_Bookcase.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_Bookcase.label</t>
+  </si>
+  <si>
+    <t>Gothicstyle Bookcase</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_Bookcase.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_Bookcase.description</t>
+  </si>
+  <si>
+    <t>A delicate bookshelf suitable for storing horror and detective novels, etc.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_BookDecoration.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_BookDecoration.label</t>
+  </si>
+  <si>
+    <t>Gothicstyle Book Decoration</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_BookDecoration.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_BookDecoration.description</t>
+  </si>
+  <si>
+    <t>Attention: After reading the books in the library, please put them back in their original positions. Management personnel usually sort out the unreturned books at midnight.</t>
+  </si>
+  <si>
+    <t>주의: 도서관에서 책을 읽은 후에는 원래 자리에 돌려놔 주세요. 제자리에 돌려놓지 않은 책은 보통 관리 직원들이 자정에 정리합니다.</t>
+  </si>
+  <si>
+    <t>고딕 책 장식</t>
+  </si>
+  <si>
+    <t>공포 소설, 추리 소설 등을 보관하기에 적합한 세련된 책장입니다.</t>
+  </si>
+  <si>
+    <t>고딕 책장</t>
+  </si>
+  <si>
+    <t>오래 전 실종된 화가가 그린 단조로운 정물화입니다. 이 그림이 걸린 방에서 지내는 방문객들은 항상 무언가가 자신을 지켜보고 있는 것 같다는 불평을 하곤 합니다.</t>
+  </si>
+  <si>
+    <t>고딕 섬뜩한 유화 액자</t>
+  </si>
+  <si>
+    <t>더 작고 가볍고, 더 경제적이고, 햇빛에 노출될 확률도 50% 더 높은 커튼입니다.</t>
+  </si>
+  <si>
+    <t>고딕 소형 커튼</t>
+  </si>
+  <si>
+    <t>우리 안의 이상한 생물체는 빨간 빛을 내는 눈을 깜박이며 우리를 흔들고 삐걱거리는 소리를 냅니다.</t>
+  </si>
+  <si>
+    <t>고딕 천장 장식</t>
+  </si>
+  <si>
+    <t>매우 무겁지만 기계 장비가 내장되어 있어 문을 여는 사람의 부담을 크게 덜 수 있습니다.</t>
+  </si>
+  <si>
+    <t>고딕 성 자동문</t>
+  </si>
+  <si>
+    <t>강철로 보강된 무거운 성문입니다.</t>
+  </si>
+  <si>
+    <t>고딕 성문</t>
+  </si>
+  <si>
+    <t>"물론, 뱀파이어 능력 같은 게 아니라 전기로 움직이는 문이지."</t>
+  </si>
+  <si>
+    <t>고딕 자동문</t>
+  </si>
+  <si>
+    <t>덤불로 장식된 아치입니다. 거대한 장미 미로 속에서 길을 잃은 사람들을 안내하는 역할을 합니다.</t>
+  </si>
+  <si>
+    <t>고딕 안뜰 아치</t>
+  </si>
+  <si>
+    <t>하중을 잘 견디는 소형 고딕식 아치입니다. 벽의 장식부로서 천장을 받칠 수는 없습니다.</t>
+  </si>
+  <si>
+    <t>고딕 소형 아치</t>
+  </si>
+  <si>
+    <t>장식, 침입 방어, 이동 통제 등 여러 용도로 쓰일 수 있는 방어벽입니다.</t>
+  </si>
+  <si>
+    <t>고딕 성 방어벽</t>
+  </si>
+  <si>
+    <t>장미처럼 생긴 꽃을 피우는 빽빽하고 튼튼한 관목입니다. 뒤에 숨어 몸을 숨기는 데도 좋지만, 장미의 미로에 갖힌 채로 불타 죽지 않도록 주의하세요.</t>
+  </si>
+  <si>
+    <t>고딕 장미 생울타리</t>
+  </si>
+  <si>
+    <t>붉은 생울타리가 안뜰을 오싹한 미로로 둘러쌌습니다.</t>
+  </si>
+  <si>
+    <t>고딕 생울타리</t>
+  </si>
+  <si>
+    <t>기둥과 부조로 장식된 고딕식 벽입니다. 창문이 달려 있어 밖을 보거나 벽 너머로 사격할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>고딕 총안구</t>
   </si>
 </sst>
 </file>
@@ -1752,10 +2088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F122"/>
+  <dimension ref="A1:F150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1764,9 +2100,10 @@
     <col min="2" max="2" width="31.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7265625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="43.90625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -1803,2047 +2140,2523 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>454</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>453</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>452</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>455</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>451</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>450</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>429</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>428</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>427</v>
+        <v>567</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>426</v>
+        <v>566</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>425</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>424</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>423</v>
+        <v>565</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>421</v>
+        <v>564</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>422</v>
+        <v>563</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>421</v>
+        <v>562</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>420</v>
+        <v>561</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>419</v>
+        <v>560</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>418</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>417</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>416</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>415</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>414</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>413</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>412</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>410</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>411</v>
+        <v>559</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>410</v>
+        <v>558</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>409</v>
+        <v>557</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>408</v>
+        <v>556</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>407</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>406</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>405</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>401</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>404</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>401</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>403</v>
+        <v>555</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>401</v>
+        <v>554</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>402</v>
+        <v>553</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>401</v>
+        <v>552</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>400</v>
+        <v>551</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>399</v>
+        <v>550</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>443</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>449</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>443</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>143</v>
+        <v>173</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>448</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>146</v>
+        <v>175</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>443</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>148</v>
+        <v>179</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>149</v>
+        <v>180</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>447</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>152</v>
+        <v>184</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>137</v>
+        <v>185</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>443</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>154</v>
+        <v>188</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>446</v>
+        <v>190</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>137</v>
+        <v>193</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>443</v>
+        <v>194</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>158</v>
+        <v>195</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>159</v>
+        <v>196</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>445</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>161</v>
+        <v>199</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>137</v>
+        <v>201</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>443</v>
+        <v>549</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>165</v>
+        <v>204</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>444</v>
+        <v>548</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>166</v>
+        <v>205</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>168</v>
+        <v>207</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>436</v>
+        <v>208</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>169</v>
+        <v>209</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>170</v>
+        <v>210</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>442</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>172</v>
+        <v>211</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>173</v>
+        <v>212</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>436</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>175</v>
+        <v>216</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>441</v>
+        <v>198</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>177</v>
+        <v>217</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>178</v>
+        <v>218</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>168</v>
+        <v>219</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>436</v>
+        <v>220</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>179</v>
+        <v>221</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>180</v>
+        <v>222</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>440</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>182</v>
+        <v>223</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>183</v>
+        <v>224</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>168</v>
+        <v>225</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>436</v>
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>184</v>
+        <v>227</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>185</v>
+        <v>228</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>186</v>
+        <v>229</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>439</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>187</v>
+        <v>231</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>188</v>
+        <v>233</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>168</v>
+        <v>234</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>436</v>
+        <v>235</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>189</v>
+        <v>236</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>190</v>
+        <v>237</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>191</v>
+        <v>238</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>438</v>
+        <v>239</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>192</v>
+        <v>240</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>193</v>
+        <v>241</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>168</v>
+        <v>234</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>436</v>
+        <v>235</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>194</v>
+        <v>242</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>195</v>
+        <v>243</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>196</v>
+        <v>244</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>437</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>197</v>
+        <v>246</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>198</v>
+        <v>247</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>199</v>
+        <v>234</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>430</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>200</v>
+        <v>248</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>201</v>
+        <v>249</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>202</v>
+        <v>250</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>435</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>203</v>
+        <v>252</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>204</v>
+        <v>253</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>199</v>
+        <v>234</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>430</v>
+        <v>235</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>205</v>
+        <v>254</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>206</v>
+        <v>255</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>207</v>
+        <v>256</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>434</v>
+        <v>257</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>208</v>
+        <v>258</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>209</v>
+        <v>259</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>199</v>
+        <v>234</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>430</v>
+        <v>235</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>210</v>
+        <v>260</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>212</v>
+        <v>262</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>433</v>
+        <v>263</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>213</v>
+        <v>264</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>214</v>
+        <v>265</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>199</v>
+        <v>234</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>430</v>
+        <v>235</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>215</v>
+        <v>266</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>216</v>
+        <v>267</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>217</v>
+        <v>268</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>432</v>
+        <v>269</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>218</v>
+        <v>270</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>199</v>
+        <v>272</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>430</v>
+        <v>273</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>220</v>
+        <v>274</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>221</v>
+        <v>275</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>222</v>
+        <v>276</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>431</v>
+        <v>277</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
-        <v>223</v>
+        <v>278</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>224</v>
+        <v>279</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>225</v>
+        <v>272</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>398</v>
+        <v>273</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>226</v>
+        <v>280</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>227</v>
+        <v>281</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>228</v>
+        <v>282</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>397</v>
+        <v>283</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>229</v>
+        <v>284</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>230</v>
+        <v>285</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>231</v>
+        <v>272</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>396</v>
+        <v>273</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="C82" s="1" t="s">
-        <v>233</v>
+        <v>287</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>234</v>
+        <v>288</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>395</v>
+        <v>289</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
-        <v>235</v>
+        <v>290</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>236</v>
+        <v>291</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>237</v>
+        <v>272</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>394</v>
+        <v>273</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
-        <v>238</v>
+        <v>292</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>239</v>
+        <v>293</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>240</v>
+        <v>294</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>393</v>
+        <v>295</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>241</v>
+        <v>296</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>242</v>
+        <v>297</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>243</v>
+        <v>272</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>392</v>
+        <v>273</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>244</v>
+        <v>298</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>245</v>
+        <v>299</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>246</v>
+        <v>300</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>391</v>
+        <v>301</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
-        <v>247</v>
+        <v>302</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>248</v>
+        <v>303</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>249</v>
+        <v>272</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>390</v>
+        <v>273</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
-        <v>250</v>
+        <v>304</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>251</v>
+        <v>305</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>252</v>
+        <v>306</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>389</v>
+        <v>307</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
-        <v>253</v>
+        <v>308</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>254</v>
+        <v>309</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>255</v>
+        <v>310</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>388</v>
+        <v>311</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
-        <v>256</v>
+        <v>312</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>257</v>
+        <v>313</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>258</v>
+        <v>314</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>387</v>
+        <v>315</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
-        <v>259</v>
+        <v>316</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>260</v>
+        <v>317</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>261</v>
+        <v>310</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>386</v>
+        <v>311</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
-        <v>262</v>
+        <v>318</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>263</v>
+        <v>319</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>264</v>
+        <v>320</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>385</v>
+        <v>321</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
-        <v>265</v>
+        <v>322</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>266</v>
+        <v>323</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>267</v>
+        <v>310</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>384</v>
+        <v>311</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
-        <v>268</v>
+        <v>324</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>269</v>
+        <v>325</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>270</v>
+        <v>326</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>383</v>
+        <v>327</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
-        <v>271</v>
+        <v>328</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>272</v>
+        <v>329</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>273</v>
+        <v>310</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>382</v>
+        <v>311</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
-        <v>274</v>
+        <v>330</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>275</v>
+        <v>331</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>276</v>
+        <v>332</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>381</v>
+        <v>333</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
-        <v>277</v>
+        <v>334</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>278</v>
+        <v>335</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>279</v>
+        <v>310</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>380</v>
+        <v>311</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
-        <v>280</v>
+        <v>336</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>281</v>
+        <v>337</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>282</v>
+        <v>338</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>379</v>
+        <v>339</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="1" t="s">
-        <v>283</v>
+        <v>340</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>284</v>
+        <v>341</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>285</v>
+        <v>342</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>378</v>
+        <v>343</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
-        <v>286</v>
+        <v>344</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>287</v>
+        <v>345</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>288</v>
+        <v>346</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
-        <v>289</v>
+        <v>348</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>290</v>
+        <v>349</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>291</v>
+        <v>350</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>376</v>
+        <v>351</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
-        <v>292</v>
+        <v>352</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>293</v>
+        <v>353</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>294</v>
+        <v>354</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>375</v>
+        <v>355</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
-        <v>295</v>
+        <v>356</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>296</v>
+        <v>357</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>297</v>
+        <v>358</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
-        <v>298</v>
+        <v>360</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>299</v>
+        <v>361</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>300</v>
+        <v>362</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
-        <v>301</v>
+        <v>364</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>302</v>
+        <v>365</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>303</v>
+        <v>366</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>372</v>
+        <v>547</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
-        <v>304</v>
+        <v>367</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>305</v>
+        <v>368</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>306</v>
+        <v>369</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>371</v>
+        <v>546</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
-        <v>307</v>
+        <v>370</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>308</v>
+        <v>371</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>309</v>
+        <v>372</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="s">
-        <v>310</v>
+        <v>374</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>311</v>
+        <v>375</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>312</v>
+        <v>376</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" s="1" t="s">
-        <v>313</v>
+        <v>378</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>314</v>
+        <v>379</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>315</v>
+        <v>380</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>368</v>
+        <v>381</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" s="1" t="s">
-        <v>316</v>
+        <v>382</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>317</v>
+        <v>383</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>318</v>
+        <v>384</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>367</v>
+        <v>385</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="s">
-        <v>319</v>
+        <v>386</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>320</v>
+        <v>387</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>321</v>
+        <v>388</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>366</v>
+        <v>389</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112" s="1" t="s">
-        <v>322</v>
+        <v>390</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>323</v>
+        <v>391</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>324</v>
+        <v>392</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>365</v>
+        <v>393</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="s">
-        <v>325</v>
+        <v>394</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>326</v>
+        <v>395</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>327</v>
+        <v>396</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>364</v>
+        <v>397</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="s">
-        <v>328</v>
+        <v>398</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>329</v>
+        <v>399</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>330</v>
+        <v>400</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>363</v>
+        <v>401</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
-        <v>331</v>
+        <v>402</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>332</v>
+        <v>403</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>333</v>
+        <v>404</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>362</v>
+        <v>545</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116" s="1" t="s">
-        <v>334</v>
+        <v>405</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>335</v>
+        <v>406</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>336</v>
+        <v>407</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>361</v>
+        <v>544</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="s">
-        <v>337</v>
+        <v>408</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>338</v>
+        <v>409</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>339</v>
+        <v>410</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>360</v>
+        <v>411</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118" s="1" t="s">
-        <v>340</v>
+        <v>412</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>341</v>
+        <v>413</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>342</v>
+        <v>414</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>359</v>
+        <v>415</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119" s="1" t="s">
-        <v>343</v>
+        <v>416</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>344</v>
+        <v>417</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>345</v>
+        <v>418</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>358</v>
+        <v>419</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120" s="1" t="s">
-        <v>346</v>
+        <v>420</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>347</v>
+        <v>421</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>348</v>
+        <v>422</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>357</v>
+        <v>423</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121" s="1" t="s">
-        <v>349</v>
+        <v>424</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>350</v>
+        <v>425</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>351</v>
+        <v>426</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>356</v>
+        <v>427</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122" s="1" t="s">
-        <v>352</v>
+        <v>428</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>353</v>
+        <v>429</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>354</v>
+        <v>430</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>355</v>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A123" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A124" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A125" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A126" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A127" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A128" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A129" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A130" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A131" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A132" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A133" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A134" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A135" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A136" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A137" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A138" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A139" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A140" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A141" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A142" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A143" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A144" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A145" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A146" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A147" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A148" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A149" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A150" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[MUS]哥特式吸血鬼家具 Gothicstyle Vampire Furniture 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/[MUS]哥特式吸血鬼家具 Gothicstyle Vampire Furniture - 3102678787/3102678787.xlsx
+++ b/Data/[MUS]哥特式吸血鬼家具 Gothicstyle Vampire Furniture - 3102678787/3102678787.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\[MUS]哥特式吸血鬼家具 Gothicstyle Vampire Furniture - 3102678787\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\RMK\Data\[MUS]哥特式吸血鬼家具 Gothicstyle Vampire Furniture - 3102678787\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27813FB3-5392-4088-86C8-A87659635D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1F05E4-714D-44A2-BA16-FD9BDF22E379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240430" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_250701" sheetId="3" r:id="rId1"/>
+    <sheet name="Old_240430" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="580">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1737,6 +1738,42 @@
   </si>
   <si>
     <t>고딕 총안구</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_MonsterStatueLarge.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_MonsterStatueLarge.label</t>
+  </si>
+  <si>
+    <t>고딕 괴수상</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_MonsterStatueLarge.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_MonsterStatueLarge.description</t>
+  </si>
+  <si>
+    <t>전설적인 괴수를 본따 만든 형상의 기이한 조각상입니다. 물론 주인의 취향에 이의를 제기할 사람은 아무도 없을 것입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_PottedPlants.label</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_PottedPlants.label</t>
+  </si>
+  <si>
+    <t>고딕 화분식물</t>
+  </si>
+  <si>
+    <t>ThingDef+MUS_Gothicstyle_PottedPlants.description</t>
+  </si>
+  <si>
+    <t>MUS_Gothicstyle_PottedPlants.description</t>
+  </si>
+  <si>
+    <t>물이나 햇빛 없이도 만개할 수 있는 이국적인 매력이 가득한 신기한 화분 식물들입니다.</t>
   </si>
 </sst>
 </file>
@@ -2087,26 +2124,2660 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9AC4E38-3AF2-4217-AF7C-B117ED834F4A}">
+  <dimension ref="A1:F155"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A173" sqref="A173"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="61.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A145" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A147" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.90625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="47.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="1"/>
+    <col min="4" max="4" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2126,7 +4797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2143,7 +4814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2160,7 +4831,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2177,7 +4848,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -2194,7 +4865,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2211,7 +4882,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -2228,7 +4899,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -2245,7 +4916,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -2262,7 +4933,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -2279,7 +4950,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -2296,7 +4967,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -2313,7 +4984,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -2330,7 +5001,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -2347,7 +5018,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
@@ -2364,7 +5035,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>62</v>
       </c>
@@ -2381,7 +5052,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -2398,7 +5069,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
@@ -2415,7 +5086,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -2432,7 +5103,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>74</v>
       </c>
@@ -2449,7 +5120,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -2466,7 +5137,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>81</v>
       </c>
@@ -2483,7 +5154,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>85</v>
       </c>
@@ -2500,7 +5171,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>89</v>
       </c>
@@ -2517,7 +5188,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>93</v>
       </c>
@@ -2534,7 +5205,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>97</v>
       </c>
@@ -2551,7 +5222,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>99</v>
       </c>
@@ -2568,7 +5239,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>103</v>
       </c>
@@ -2585,7 +5256,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>107</v>
       </c>
@@ -2602,7 +5273,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>110</v>
       </c>
@@ -2619,7 +5290,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>113</v>
       </c>
@@ -2636,7 +5307,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>116</v>
       </c>
@@ -2653,7 +5324,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>119</v>
       </c>
@@ -2670,7 +5341,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>123</v>
       </c>
@@ -2687,7 +5358,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>127</v>
       </c>
@@ -2704,7 +5375,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>131</v>
       </c>
@@ -2721,7 +5392,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>135</v>
       </c>
@@ -2738,7 +5409,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>139</v>
       </c>
@@ -2755,7 +5426,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>143</v>
       </c>
@@ -2772,7 +5443,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>146</v>
       </c>
@@ -2789,7 +5460,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>149</v>
       </c>
@@ -2806,7 +5477,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>152</v>
       </c>
@@ -2823,7 +5494,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>155</v>
       </c>
@@ -2840,7 +5511,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>158</v>
       </c>
@@ -2857,7 +5528,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>161</v>
       </c>
@@ -2874,7 +5545,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>165</v>
       </c>
@@ -2891,7 +5562,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>169</v>
       </c>
@@ -2908,7 +5579,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>173</v>
       </c>
@@ -2925,7 +5596,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>175</v>
       </c>
@@ -2942,7 +5613,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>179</v>
       </c>
@@ -2959,7 +5630,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>183</v>
       </c>
@@ -2976,7 +5647,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>187</v>
       </c>
@@ -2993,7 +5664,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>191</v>
       </c>
@@ -3010,7 +5681,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>195</v>
       </c>
@@ -3027,7 +5698,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>199</v>
       </c>
@@ -3044,7 +5715,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>202</v>
       </c>
@@ -3061,7 +5732,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>205</v>
       </c>
@@ -3078,7 +5749,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>209</v>
       </c>
@@ -3095,7 +5766,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>211</v>
       </c>
@@ -3112,7 +5783,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>215</v>
       </c>
@@ -3129,7 +5800,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>217</v>
       </c>
@@ -3146,7 +5817,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>221</v>
       </c>
@@ -3163,7 +5834,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>223</v>
       </c>
@@ -3180,7 +5851,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>227</v>
       </c>
@@ -3197,7 +5868,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>231</v>
       </c>
@@ -3214,7 +5885,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>236</v>
       </c>
@@ -3231,7 +5902,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>240</v>
       </c>
@@ -3248,7 +5919,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>242</v>
       </c>
@@ -3265,7 +5936,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>246</v>
       </c>
@@ -3282,7 +5953,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>248</v>
       </c>
@@ -3299,7 +5970,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>252</v>
       </c>
@@ -3316,7 +5987,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>254</v>
       </c>
@@ -3333,7 +6004,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>258</v>
       </c>
@@ -3350,7 +6021,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>260</v>
       </c>
@@ -3367,7 +6038,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>264</v>
       </c>
@@ -3384,7 +6055,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>266</v>
       </c>
@@ -3401,7 +6072,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>270</v>
       </c>
@@ -3418,7 +6089,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>274</v>
       </c>
@@ -3435,7 +6106,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>278</v>
       </c>
@@ -3452,7 +6123,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>280</v>
       </c>
@@ -3469,7 +6140,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>284</v>
       </c>
@@ -3486,7 +6157,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>286</v>
       </c>
@@ -3503,7 +6174,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>290</v>
       </c>
@@ -3520,7 +6191,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>292</v>
       </c>
@@ -3537,7 +6208,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>296</v>
       </c>
@@ -3554,7 +6225,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>298</v>
       </c>
@@ -3571,7 +6242,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>302</v>
       </c>
@@ -3588,7 +6259,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>304</v>
       </c>
@@ -3605,7 +6276,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>308</v>
       </c>
@@ -3622,7 +6293,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>312</v>
       </c>
@@ -3639,7 +6310,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>316</v>
       </c>
@@ -3656,7 +6327,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>318</v>
       </c>
@@ -3673,7 +6344,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>322</v>
       </c>
@@ -3690,7 +6361,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>324</v>
       </c>
@@ -3707,7 +6378,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>328</v>
       </c>
@@ -3724,7 +6395,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>330</v>
       </c>
@@ -3741,7 +6412,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>334</v>
       </c>
@@ -3758,7 +6429,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>336</v>
       </c>
@@ -3775,7 +6446,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>340</v>
       </c>
@@ -3792,7 +6463,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>344</v>
       </c>
@@ -3809,7 +6480,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>348</v>
       </c>
@@ -3826,7 +6497,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>352</v>
       </c>
@@ -3843,7 +6514,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>356</v>
       </c>
@@ -3860,7 +6531,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>360</v>
       </c>
@@ -3877,7 +6548,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>364</v>
       </c>
@@ -3894,7 +6565,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>367</v>
       </c>
@@ -3911,7 +6582,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>370</v>
       </c>
@@ -3928,7 +6599,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>374</v>
       </c>
@@ -3945,7 +6616,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>378</v>
       </c>
@@ -3962,7 +6633,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>382</v>
       </c>
@@ -3979,7 +6650,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>386</v>
       </c>
@@ -3996,7 +6667,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>390</v>
       </c>
@@ -4013,7 +6684,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>394</v>
       </c>
@@ -4030,7 +6701,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>398</v>
       </c>
@@ -4047,7 +6718,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>402</v>
       </c>
@@ -4064,7 +6735,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>405</v>
       </c>
@@ -4081,7 +6752,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>408</v>
       </c>
@@ -4098,7 +6769,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>412</v>
       </c>
@@ -4115,7 +6786,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>416</v>
       </c>
@@ -4132,7 +6803,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>420</v>
       </c>
@@ -4149,7 +6820,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>424</v>
       </c>
@@ -4166,7 +6837,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>428</v>
       </c>
@@ -4183,7 +6854,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>432</v>
       </c>
@@ -4200,7 +6871,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>436</v>
       </c>
@@ -4217,7 +6888,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>440</v>
       </c>
@@ -4234,7 +6905,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>444</v>
       </c>
@@ -4251,7 +6922,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>448</v>
       </c>
@@ -4268,7 +6939,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>452</v>
       </c>
@@ -4285,7 +6956,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>456</v>
       </c>
@@ -4302,7 +6973,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>460</v>
       </c>
@@ -4319,7 +6990,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>464</v>
       </c>
@@ -4336,7 +7007,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>468</v>
       </c>
@@ -4353,7 +7024,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>472</v>
       </c>
@@ -4370,7 +7041,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>476</v>
       </c>
@@ -4387,7 +7058,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>480</v>
       </c>
@@ -4404,7 +7075,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>484</v>
       </c>
@@ -4421,7 +7092,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>488</v>
       </c>
@@ -4438,7 +7109,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>492</v>
       </c>
@@ -4455,7 +7126,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>496</v>
       </c>
@@ -4472,7 +7143,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>500</v>
       </c>
@@ -4489,7 +7160,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>504</v>
       </c>
@@ -4506,7 +7177,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>508</v>
       </c>
@@ -4523,7 +7194,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>512</v>
       </c>
@@ -4540,7 +7211,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>516</v>
       </c>
@@ -4557,7 +7228,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>520</v>
       </c>
@@ -4574,7 +7245,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>524</v>
       </c>
@@ -4591,7 +7262,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>528</v>
       </c>
@@ -4608,7 +7279,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>531</v>
       </c>
@@ -4625,7 +7296,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>534</v>
       </c>
@@ -4642,7 +7313,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>537</v>
       </c>

</xml_diff>